<commit_message>
finished lowpass filter and linear fit
</commit_message>
<xml_diff>
--- a/Senior design/Raw Data/4 types 12-19 points.xlsx
+++ b/Senior design/Raw Data/4 types 12-19 points.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="4 Small Sets" sheetId="1" r:id="rId1"/>
     <sheet name="large set with kgf and Nm" sheetId="2" r:id="rId2"/>
     <sheet name="Results Algorithm" sheetId="3" r:id="rId3"/>
+    <sheet name="Graph Data" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>10 mile TT</t>
   </si>
@@ -96,6 +97,18 @@
   <si>
     <t>Optimal time: (do nothing/new time)*100</t>
   </si>
+  <si>
+    <t>Raw Data sample</t>
+  </si>
+  <si>
+    <t>Raw Data - Bad Data</t>
+  </si>
+  <si>
+    <t>Low Pass fill</t>
+  </si>
+  <si>
+    <t>Linear fit</t>
+  </si>
 </sst>
 </file>
 
@@ -110,12 +123,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -158,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -166,11 +185,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,6 +206,3020 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Data Analysis through filters</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph Data'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw Data sample</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$B$3:$B$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$C$3:$C$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>3.34375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.46875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.78125</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.484375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.46875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.59375</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.203125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.65625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.8125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.78125</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.40625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.03125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.53125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.90625</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.84375</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.078125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.28125</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2890625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9375</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.90625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.453125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.46875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.96875</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.671875</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.21875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0625</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.96875</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.71875</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.9375</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.40625</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>12.6875</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>13.90625</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.109375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>16.625</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>17.40625</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8828125</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>19.59375</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>18.96875</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.734375</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>16.90625</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>16.65625</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>15.15625</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>14.34375</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>13.1875</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.5625</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.9375</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.328125</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.9375</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.203125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-822F-453B-B27E-A64354A42A93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph Data'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Raw Data - Bad Data</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$B$3:$B$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$D$3:$D$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>3.34375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.46875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.484375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.203125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.65625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.8125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.78125</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.40625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.03125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.53125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.90625</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.84375</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.078125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.28125</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2890625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9375</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.90625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.453125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.46875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.96875</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.671875</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.21875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0625</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.96875</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.71875</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.9375</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.40625</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.109375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8828125</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.734375</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.5625</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.9375</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.328125</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.9375</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.203125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-822F-453B-B27E-A64354A42A93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph Data'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Low Pass fill</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$B$3:$B$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$E$3:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>3.34375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.46875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.140625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.15234375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.484375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.9386718749999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8648082386363596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.203125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.65625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.8125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.78125</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.40625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.03125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.53125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.90625</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.84375</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.078125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.28125</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2890625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9375</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.90625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.453125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.46875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.96875</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.671875</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.21875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0625</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.96875</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.71875</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.9375</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.40625</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.2301136363636296</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.0095557851239603</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.109375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>7.2171006292261399</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>7.9527461409739697</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8828125</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>8.9129389719716094</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>8.9391152421508497</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.734375</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.2933426608587695</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.43277783138012</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9.8856234861213892</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.7346350629529699</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>9.77514165958506</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.5625</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.9375</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.328125</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.9375</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.203125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-822F-453B-B27E-A64354A42A93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graph Data'!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear fit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$B$3:$B$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Graph Data'!$F$3:$F$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>3.34375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.46875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0486042080848197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8974967773623597</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.484375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.2902881766350403</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.3026284677718198</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.203125</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.65625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.8125</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.78125</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.40625</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.03125</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.53125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.90625</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.84375</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.078125</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.28125</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.2890625</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0625</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.9375</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.90625</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8125</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.453125</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.46875</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.96875</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1875</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.875</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.8125</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.78125</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.375</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.671875</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.21875</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.0625</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.59375</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.171875</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.9375</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.96875</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.71875</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.9375</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.40625</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.54403362380795</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>7.9462554217904096</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.109375</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>9.2158955081417009</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>10.557646480770099</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8828125</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.4035256192280903</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.0585736635881</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>8.734375</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.6429547254538797</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>10.7178530631173</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.90625</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.7483660910351997</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.71460234595766</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10.846293530165401</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.5625</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>9.9375</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.328125</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.9375</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.375</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.203125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-822F-453B-B27E-A64354A42A93}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="505500344"/>
+        <c:axId val="505500672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="505500344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505500672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="505500672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx2"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="505500344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx2">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="242">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk2">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="2"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57ED8E7F-3419-48BD-BE72-FE4149B305F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,8 +4025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:M1897"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7:I1897"/>
+    <sheetView topLeftCell="A1577" workbookViewId="0">
+      <selection activeCell="I1586" sqref="I1586:I1595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,11 +4040,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:13" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
       <c r="M2" t="s">
         <v>11</v>
       </c>
@@ -36998,7 +40032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -37011,71 +40045,71 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>257177</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>257177</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>257177</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>14960</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>29920</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>29920</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>9</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>12</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <f>$C$7/C7*100</f>
         <v>100</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <f>$C$7/D7*100</f>
         <v>75</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f>$C$7/E7*100</f>
         <v>64.285714285714292</v>
       </c>
@@ -37083,4 +40117,1484 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="O66" sqref="O66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3.34375</v>
+      </c>
+      <c r="D3">
+        <f>IF(C3&lt;12, C3, " " )</f>
+        <v>3.34375</v>
+      </c>
+      <c r="E3">
+        <v>3.34375</v>
+      </c>
+      <c r="F3">
+        <v>3.34375</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>1+B3</f>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>7.90625</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D68" si="0">IF(C4&lt;12, C4, " " )</f>
+        <v>7.90625</v>
+      </c>
+      <c r="E4">
+        <v>7.90625</v>
+      </c>
+      <c r="F4">
+        <v>7.90625</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ref="B5:B68" si="1">1+B4</f>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>8.625</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.625</v>
+      </c>
+      <c r="E5">
+        <v>8.625</v>
+      </c>
+      <c r="F5">
+        <v>8.625</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5.46875</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>5.46875</v>
+      </c>
+      <c r="E6">
+        <v>5.46875</v>
+      </c>
+      <c r="F6">
+        <v>5.46875</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>12.375</v>
+      </c>
+      <c r="D7" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E7" s="8">
+        <v>8.140625</v>
+      </c>
+      <c r="F7" s="8">
+        <v>6.0486042080848197</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C8" s="8">
+        <v>12.78125</v>
+      </c>
+      <c r="D8" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E8" s="8">
+        <v>8.15234375</v>
+      </c>
+      <c r="F8" s="8">
+        <v>6.8974967773623597</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>6.484375</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>6.484375</v>
+      </c>
+      <c r="E9">
+        <v>6.484375</v>
+      </c>
+      <c r="F9">
+        <v>6.484375</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C10" s="8">
+        <v>12.46875</v>
+      </c>
+      <c r="D10" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E10" s="8">
+        <v>7.9386718749999998</v>
+      </c>
+      <c r="F10" s="8">
+        <v>7.2902881766350403</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="8">
+        <v>12.59375</v>
+      </c>
+      <c r="D11" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E11" s="8">
+        <v>7.8648082386363596</v>
+      </c>
+      <c r="F11" s="8">
+        <v>8.3026284677718198</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>6.203125</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>6.203125</v>
+      </c>
+      <c r="E12">
+        <v>6.203125</v>
+      </c>
+      <c r="F12">
+        <v>6.203125</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>11.65625</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>11.65625</v>
+      </c>
+      <c r="E13">
+        <v>11.65625</v>
+      </c>
+      <c r="F13">
+        <v>11.65625</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>10.8125</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>10.8125</v>
+      </c>
+      <c r="E14">
+        <v>10.8125</v>
+      </c>
+      <c r="F14">
+        <v>10.8125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>4.75</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="E15">
+        <v>4.75</v>
+      </c>
+      <c r="F15">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>8.78125</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>8.78125</v>
+      </c>
+      <c r="E17">
+        <v>8.78125</v>
+      </c>
+      <c r="F17">
+        <v>8.78125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>8.40625</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>8.40625</v>
+      </c>
+      <c r="E18">
+        <v>8.40625</v>
+      </c>
+      <c r="F18">
+        <v>8.40625</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>7.90625</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>7.90625</v>
+      </c>
+      <c r="E19">
+        <v>7.90625</v>
+      </c>
+      <c r="F19">
+        <v>7.90625</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>7.03125</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>7.03125</v>
+      </c>
+      <c r="E20">
+        <v>7.03125</v>
+      </c>
+      <c r="F20">
+        <v>7.03125</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>2.53125</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>2.53125</v>
+      </c>
+      <c r="E21">
+        <v>2.53125</v>
+      </c>
+      <c r="F21">
+        <v>2.53125</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>4.90625</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>4.90625</v>
+      </c>
+      <c r="E22">
+        <v>4.90625</v>
+      </c>
+      <c r="F22">
+        <v>4.90625</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>3.84375</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3.84375</v>
+      </c>
+      <c r="E23">
+        <v>3.84375</v>
+      </c>
+      <c r="F23">
+        <v>3.84375</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>1.078125</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1.078125</v>
+      </c>
+      <c r="E24">
+        <v>1.078125</v>
+      </c>
+      <c r="F24">
+        <v>1.078125</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>1.28125</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1.28125</v>
+      </c>
+      <c r="E25">
+        <v>1.28125</v>
+      </c>
+      <c r="F25">
+        <v>1.28125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>0.2890625</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0.2890625</v>
+      </c>
+      <c r="E27">
+        <v>0.2890625</v>
+      </c>
+      <c r="F27">
+        <v>0.2890625</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>2.0625</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2.0625</v>
+      </c>
+      <c r="E28">
+        <v>2.0625</v>
+      </c>
+      <c r="F28">
+        <v>2.0625</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>2.9375</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2.9375</v>
+      </c>
+      <c r="E29">
+        <v>2.9375</v>
+      </c>
+      <c r="F29">
+        <v>2.9375</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>1.5</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E30">
+        <v>1.5</v>
+      </c>
+      <c r="F30">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>2.90625</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>2.90625</v>
+      </c>
+      <c r="E31">
+        <v>2.90625</v>
+      </c>
+      <c r="F31">
+        <v>2.90625</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>2.8125</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>2.8125</v>
+      </c>
+      <c r="E32">
+        <v>2.8125</v>
+      </c>
+      <c r="F32">
+        <v>2.8125</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>1.453125</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1.453125</v>
+      </c>
+      <c r="E33">
+        <v>1.453125</v>
+      </c>
+      <c r="F33">
+        <v>1.453125</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>2.75</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="E34">
+        <v>2.75</v>
+      </c>
+      <c r="F34">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>2.09375</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>2.09375</v>
+      </c>
+      <c r="E35">
+        <v>2.09375</v>
+      </c>
+      <c r="F35">
+        <v>2.09375</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>1.46875</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>1.46875</v>
+      </c>
+      <c r="E36">
+        <v>1.46875</v>
+      </c>
+      <c r="F36">
+        <v>1.46875</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>0.96875</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>0.96875</v>
+      </c>
+      <c r="E37">
+        <v>0.96875</v>
+      </c>
+      <c r="F37">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>1.1875</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>1.1875</v>
+      </c>
+      <c r="E38">
+        <v>1.1875</v>
+      </c>
+      <c r="F38">
+        <v>1.1875</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>0.875</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>0.875</v>
+      </c>
+      <c r="E40">
+        <v>0.875</v>
+      </c>
+      <c r="F40">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <v>0.8125</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>0.8125</v>
+      </c>
+      <c r="E41">
+        <v>0.8125</v>
+      </c>
+      <c r="F41">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>0.375</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="E42">
+        <v>0.375</v>
+      </c>
+      <c r="F42">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <v>0.78125</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>0.78125</v>
+      </c>
+      <c r="E43">
+        <v>0.78125</v>
+      </c>
+      <c r="F43">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>1.375</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>1.375</v>
+      </c>
+      <c r="E44">
+        <v>1.375</v>
+      </c>
+      <c r="F44">
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>0.671875</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>0.671875</v>
+      </c>
+      <c r="E45">
+        <v>0.671875</v>
+      </c>
+      <c r="F45">
+        <v>0.671875</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>1.5</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="E46">
+        <v>1.5</v>
+      </c>
+      <c r="F46">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>1.21875</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>1.21875</v>
+      </c>
+      <c r="E47">
+        <v>1.21875</v>
+      </c>
+      <c r="F47">
+        <v>1.21875</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>0.75</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="E48">
+        <v>0.75</v>
+      </c>
+      <c r="F48">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>1.0625</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>1.0625</v>
+      </c>
+      <c r="E49">
+        <v>1.0625</v>
+      </c>
+      <c r="F49">
+        <v>1.0625</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="C50">
+        <v>0.59375</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>0.59375</v>
+      </c>
+      <c r="E50">
+        <v>0.59375</v>
+      </c>
+      <c r="F50">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>0.171875</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>0.171875</v>
+      </c>
+      <c r="E51">
+        <v>0.171875</v>
+      </c>
+      <c r="F51">
+        <v>0.171875</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>0.9375</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>0.9375</v>
+      </c>
+      <c r="E52">
+        <v>0.9375</v>
+      </c>
+      <c r="F52">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="C53">
+        <v>2.09375</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>2.09375</v>
+      </c>
+      <c r="E53">
+        <v>2.09375</v>
+      </c>
+      <c r="F53">
+        <v>2.09375</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="C54">
+        <v>2.96875</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>2.96875</v>
+      </c>
+      <c r="E54">
+        <v>2.96875</v>
+      </c>
+      <c r="F54">
+        <v>2.96875</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="C55">
+        <v>4.71875</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>4.71875</v>
+      </c>
+      <c r="E55">
+        <v>4.71875</v>
+      </c>
+      <c r="F55">
+        <v>4.71875</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="C56">
+        <v>5.9375</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>5.9375</v>
+      </c>
+      <c r="E56">
+        <v>5.9375</v>
+      </c>
+      <c r="F56">
+        <v>5.9375</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="C57">
+        <v>5.40625</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>5.40625</v>
+      </c>
+      <c r="E57">
+        <v>5.40625</v>
+      </c>
+      <c r="F57">
+        <v>5.40625</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="C58" s="8">
+        <v>12.6875</v>
+      </c>
+      <c r="D58" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E58" s="8">
+        <v>5.2301136363636296</v>
+      </c>
+      <c r="F58" s="8">
+        <v>6.54403362380795</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="C59" s="8">
+        <v>13.90625</v>
+      </c>
+      <c r="D59" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E59" s="8">
+        <v>6.0095557851239603</v>
+      </c>
+      <c r="F59" s="8">
+        <v>7.9462554217904096</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>8.109375</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>8.109375</v>
+      </c>
+      <c r="E60">
+        <v>8.109375</v>
+      </c>
+      <c r="F60">
+        <v>8.109375</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="C61" s="8">
+        <v>16.625</v>
+      </c>
+      <c r="D61" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E61" s="8">
+        <v>7.2171006292261399</v>
+      </c>
+      <c r="F61" s="8">
+        <v>9.2158955081417009</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="C62" s="8">
+        <v>17.40625</v>
+      </c>
+      <c r="D62" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E62" s="8">
+        <v>7.9527461409739697</v>
+      </c>
+      <c r="F62" s="8">
+        <v>10.557646480770099</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>4.8828125</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>4.8828125</v>
+      </c>
+      <c r="E63">
+        <v>4.8828125</v>
+      </c>
+      <c r="F63">
+        <v>4.8828125</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C64" s="8">
+        <v>19.59375</v>
+      </c>
+      <c r="D64" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E64" s="8">
+        <v>8.9129389719716094</v>
+      </c>
+      <c r="F64" s="8">
+        <v>5.4035256192280903</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="C65" s="8">
+        <v>18.96875</v>
+      </c>
+      <c r="D65" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E65" s="8">
+        <v>8.9391152421508497</v>
+      </c>
+      <c r="F65" s="8">
+        <v>6.0585736635881</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>8.734375</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>8.734375</v>
+      </c>
+      <c r="E66">
+        <v>8.734375</v>
+      </c>
+      <c r="F66">
+        <v>8.734375</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="C67" s="8">
+        <v>16.90625</v>
+      </c>
+      <c r="D67" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E67" s="8">
+        <v>9.2933426608587695</v>
+      </c>
+      <c r="F67" s="8">
+        <v>9.6429547254538797</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="C68" s="8">
+        <v>16.65625</v>
+      </c>
+      <c r="D68" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E68" s="8">
+        <v>9.43277783138012</v>
+      </c>
+      <c r="F68" s="8">
+        <v>10.7178530631173</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <f t="shared" ref="B69:B78" si="2">1+B68</f>
+        <v>67</v>
+      </c>
+      <c r="C69">
+        <v>7.90625</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ref="D69:D78" si="3">IF(C69&lt;12, C69, " " )</f>
+        <v>7.90625</v>
+      </c>
+      <c r="E69">
+        <v>7.90625</v>
+      </c>
+      <c r="F69">
+        <v>7.90625</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="C70" s="8">
+        <v>15.15625</v>
+      </c>
+      <c r="D70" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E70" s="8">
+        <v>9.8856234861213892</v>
+      </c>
+      <c r="F70" s="8">
+        <v>8.7483660910351997</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <f t="shared" si="2"/>
+        <v>69</v>
+      </c>
+      <c r="C71" s="8">
+        <v>14.34375</v>
+      </c>
+      <c r="D71" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E71" s="8">
+        <v>9.7346350629529699</v>
+      </c>
+      <c r="F71" s="8">
+        <v>9.71460234595766</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="C72" s="8">
+        <v>13.1875</v>
+      </c>
+      <c r="D72" s="8" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E72" s="8">
+        <v>9.77514165958506</v>
+      </c>
+      <c r="F72" s="8">
+        <v>10.846293530165401</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="C73">
+        <v>11.5625</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="3"/>
+        <v>11.5625</v>
+      </c>
+      <c r="E73">
+        <v>11.5625</v>
+      </c>
+      <c r="F73">
+        <v>11.5625</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="C74">
+        <v>9.9375</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="3"/>
+        <v>9.9375</v>
+      </c>
+      <c r="E74">
+        <v>9.9375</v>
+      </c>
+      <c r="F74">
+        <v>9.9375</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <f t="shared" si="2"/>
+        <v>73</v>
+      </c>
+      <c r="C75">
+        <v>3.328125</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="3"/>
+        <v>3.328125</v>
+      </c>
+      <c r="E75">
+        <v>3.328125</v>
+      </c>
+      <c r="F75">
+        <v>3.328125</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="C76">
+        <v>4.9375</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="3"/>
+        <v>4.9375</v>
+      </c>
+      <c r="E76">
+        <v>4.9375</v>
+      </c>
+      <c r="F76">
+        <v>4.9375</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="C77">
+        <v>4.375</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="3"/>
+        <v>4.375</v>
+      </c>
+      <c r="E77">
+        <v>4.375</v>
+      </c>
+      <c r="F77">
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="C78">
+        <v>1.203125</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="3"/>
+        <v>1.203125</v>
+      </c>
+      <c r="E78">
+        <v>1.203125</v>
+      </c>
+      <c r="F78">
+        <v>1.203125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding compression to data
</commit_message>
<xml_diff>
--- a/Senior design/Raw Data/4 types 12-19 points.xlsx
+++ b/Senior design/Raw Data/4 types 12-19 points.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>10 mile TT</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Linear fit</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>count=totalPoints</t>
   </si>
 </sst>
 </file>
@@ -40121,10 +40127,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F78"/>
+  <dimension ref="B2:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="O66" sqref="O66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40133,9 +40139,11 @@
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>23</v>
       </c>
@@ -40148,8 +40156,14 @@
       <c r="F2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -40166,8 +40180,11 @@
       <c r="F3">
         <v>3.34375</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>3.34375</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>1+B3</f>
         <v>2</v>
@@ -40185,8 +40202,11 @@
       <c r="F4">
         <v>7.90625</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>7.90625</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5">
         <f t="shared" ref="B5:B68" si="1">1+B4</f>
         <v>3</v>
@@ -40204,8 +40224,11 @@
       <c r="F5">
         <v>8.625</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>8.625</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -40223,8 +40246,11 @@
       <c r="F6">
         <v>5.46875</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>5.46875</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -40242,8 +40268,11 @@
       <c r="F7" s="8">
         <v>6.0486042080848197</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>8.4166666666666607</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -40261,8 +40290,11 @@
       <c r="F8" s="8">
         <v>6.8974967773623597</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>7.5751488095238004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -40280,8 +40312,11 @@
       <c r="F9">
         <v>6.484375</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>6.484375</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -40299,8 +40334,11 @@
       <c r="F10" s="8">
         <v>7.2902881766350403</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>8.0980489417989396</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -40318,8 +40356,11 @@
       <c r="F11" s="8">
         <v>8.3026284677718198</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>7.4714864417989402</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -40337,8 +40378,11 @@
       <c r="F12">
         <v>6.203125</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>6.203125</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -40356,8 +40400,11 @@
       <c r="F13">
         <v>11.65625</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>11.65625</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -40375,8 +40422,11 @@
       <c r="F14">
         <v>10.8125</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>10.8125</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -40394,8 +40444,11 @@
       <c r="F15">
         <v>4.75</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>4.75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -40413,8 +40466,11 @@
       <c r="F16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -40432,8 +40488,11 @@
       <c r="F17">
         <v>8.78125</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>8.78125</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -40451,8 +40510,11 @@
       <c r="F18">
         <v>8.40625</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>8.40625</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -40470,8 +40532,11 @@
       <c r="F19">
         <v>7.90625</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>7.90625</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20">
         <f t="shared" si="1"/>
         <v>18</v>
@@ -40489,8 +40554,11 @@
       <c r="F20">
         <v>7.03125</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>7.03125</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -40508,8 +40576,11 @@
       <c r="F21">
         <v>2.53125</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>2.53125</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -40527,8 +40598,11 @@
       <c r="F22">
         <v>4.90625</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>4.90625</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -40546,8 +40620,11 @@
       <c r="F23">
         <v>3.84375</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>3.84375</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -40565,8 +40642,11 @@
       <c r="F24">
         <v>1.078125</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>1.078125</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="1"/>
         <v>23</v>
@@ -40584,8 +40664,11 @@
       <c r="F25">
         <v>1.28125</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>1.28125</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="1"/>
         <v>24</v>
@@ -40603,8 +40686,11 @@
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="1"/>
         <v>25</v>
@@ -40622,8 +40708,11 @@
       <c r="F27">
         <v>0.2890625</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>0.2890625</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="1"/>
         <v>26</v>
@@ -40641,8 +40730,11 @@
       <c r="F28">
         <v>2.0625</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>2.0625</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="1"/>
         <v>27</v>
@@ -40660,8 +40752,11 @@
       <c r="F29">
         <v>2.9375</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>2.9375</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="1"/>
         <v>28</v>
@@ -40679,8 +40774,11 @@
       <c r="F30">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="1"/>
         <v>29</v>
@@ -40698,8 +40796,11 @@
       <c r="F31">
         <v>2.90625</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>2.90625</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -40717,8 +40818,11 @@
       <c r="F32">
         <v>2.8125</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>2.8125</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="1"/>
         <v>31</v>
@@ -40736,8 +40840,11 @@
       <c r="F33">
         <v>1.453125</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>1.453125</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="1"/>
         <v>32</v>
@@ -40755,8 +40862,11 @@
       <c r="F34">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -40774,8 +40884,11 @@
       <c r="F35">
         <v>2.09375</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>2.09375</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -40793,8 +40906,11 @@
       <c r="F36">
         <v>1.46875</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>1.46875</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -40812,8 +40928,11 @@
       <c r="F37">
         <v>0.96875</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -40831,8 +40950,11 @@
       <c r="F38">
         <v>1.1875</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>1.1875</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -40850,8 +40972,11 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -40869,8 +40994,11 @@
       <c r="F40">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -40888,8 +41016,11 @@
       <c r="F41">
         <v>0.8125</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>0.8125</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -40907,8 +41038,11 @@
       <c r="F42">
         <v>0.375</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -40926,8 +41060,11 @@
       <c r="F43">
         <v>0.78125</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>0.78125</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -40945,8 +41082,11 @@
       <c r="F44">
         <v>1.375</v>
       </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -40964,8 +41104,11 @@
       <c r="F45">
         <v>0.671875</v>
       </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <v>0.671875</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -40983,8 +41126,11 @@
       <c r="F46">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -41002,8 +41148,11 @@
       <c r="F47">
         <v>1.21875</v>
       </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <v>1.21875</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -41021,8 +41170,11 @@
       <c r="F48">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -41040,8 +41192,11 @@
       <c r="F49">
         <v>1.0625</v>
       </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <v>1.0625</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -41059,8 +41214,11 @@
       <c r="F50">
         <v>0.59375</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -41078,8 +41236,11 @@
       <c r="F51">
         <v>0.171875</v>
       </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <v>0.171875</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -41097,8 +41258,11 @@
       <c r="F52">
         <v>0.9375</v>
       </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -41116,8 +41280,11 @@
       <c r="F53">
         <v>2.09375</v>
       </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G53">
+        <v>2.09375</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -41135,8 +41302,11 @@
       <c r="F54">
         <v>2.96875</v>
       </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G54">
+        <v>2.96875</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -41154,8 +41324,11 @@
       <c r="F55">
         <v>4.71875</v>
       </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G55">
+        <v>4.71875</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="1"/>
         <v>54</v>
@@ -41173,8 +41346,11 @@
       <c r="F56">
         <v>5.9375</v>
       </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G56">
+        <v>5.9375</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -41192,8 +41368,11 @@
       <c r="F57">
         <v>5.40625</v>
       </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G57">
+        <v>5.40625</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="1"/>
         <v>56</v>
@@ -41211,8 +41390,11 @@
       <c r="F58" s="8">
         <v>6.54403362380795</v>
       </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G58">
+        <v>4.5894886363636296</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="1"/>
         <v>57</v>
@@ -41230,8 +41412,11 @@
       <c r="F59" s="8">
         <v>7.9462554217904096</v>
       </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G59">
+        <v>4.4939307851239603</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="1"/>
         <v>58</v>
@@ -41249,8 +41434,11 @@
       <c r="F60">
         <v>8.109375</v>
       </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <v>8.109375</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="1"/>
         <v>59</v>
@@ -41268,8 +41456,11 @@
       <c r="F61" s="8">
         <v>9.2158955081417009</v>
       </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G61">
+        <v>6.6624131292261399</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -41287,8 +41478,11 @@
       <c r="F62" s="8">
         <v>10.557646480770099</v>
       </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G62">
+        <v>6.11538818642852</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -41306,8 +41500,11 @@
       <c r="F63">
         <v>4.8828125</v>
       </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G63">
+        <v>4.8828125</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -41325,8 +41522,11 @@
       <c r="F64" s="8">
         <v>5.4035256192280903</v>
       </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>8.1344007488311103</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -41344,8 +41544,11 @@
       <c r="F65" s="8">
         <v>6.0585736635881</v>
       </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>7.4576985441793902</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -41363,8 +41566,11 @@
       <c r="F66">
         <v>8.734375</v>
       </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>8.734375</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="1"/>
         <v>65</v>
@@ -41382,8 +41588,11 @@
       <c r="F67" s="8">
         <v>9.6429547254538797</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>8.4311256845593405</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -41401,8 +41610,11 @@
       <c r="F68" s="8">
         <v>10.7178530631173</v>
       </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>7.9621835980316797</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" ref="B69:B78" si="2">1+B68</f>
         <v>67</v>
@@ -41420,8 +41632,11 @@
       <c r="F69">
         <v>7.90625</v>
       </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>7.90625</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="2"/>
         <v>68</v>
@@ -41439,8 +41654,11 @@
       <c r="F70" s="8">
         <v>8.7483660910351997</v>
       </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>8.7078770355687407</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="2"/>
         <v>69</v>
@@ -41458,8 +41676,11 @@
       <c r="F71" s="8">
         <v>9.71460234595766</v>
       </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>8.7148510270544293</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -41477,8 +41698,11 @@
       <c r="F72" s="8">
         <v>10.846293530165401</v>
       </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>8.6983249216567895</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="2"/>
         <v>71</v>
@@ -41496,8 +41720,11 @@
       <c r="F73">
         <v>11.5625</v>
       </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>11.5625</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="2"/>
         <v>72</v>
@@ -41515,8 +41742,11 @@
       <c r="F74">
         <v>9.9375</v>
       </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>9.9375</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="2"/>
         <v>73</v>
@@ -41534,8 +41764,11 @@
       <c r="F75">
         <v>3.328125</v>
       </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>3.328125</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="2"/>
         <v>74</v>
@@ -41553,8 +41786,11 @@
       <c r="F76">
         <v>4.9375</v>
       </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>4.9375</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="2"/>
         <v>75</v>
@@ -41572,8 +41808,11 @@
       <c r="F77">
         <v>4.375</v>
       </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>4.375</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="2"/>
         <v>76</v>
@@ -41589,6 +41828,9 @@
         <v>1.203125</v>
       </c>
       <c r="F78">
+        <v>1.203125</v>
+      </c>
+      <c r="G78">
         <v>1.203125</v>
       </c>
     </row>

</xml_diff>